<commit_message>
add alternative names, readme hyperlinks
</commit_message>
<xml_diff>
--- a/uniprotDataScript/input_files/fields.xlsx
+++ b/uniprotDataScript/input_files/fields.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\David Huang\PycharmProjects\pythonProject\input_files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\David Huang\PycharmProjects\webGlycoEnzDB\uniprotDataScript\input_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9828901F-DFFC-4F13-B26B-963868941E7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92937615-C948-4600-98A2-820B458445E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{5F3E80C5-809F-48DF-852F-89AEB1066676}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
   <si>
     <t>Gene Name</t>
   </si>
@@ -55,9 +55,6 @@
     <t>HGNC number</t>
   </si>
   <si>
-    <t>OMIN-Gene</t>
-  </si>
-  <si>
     <t>Catalytic: EC</t>
   </si>
   <si>
@@ -92,6 +89,12 @@
   </si>
   <si>
     <t xml:space="preserve">Shorted </t>
+  </si>
+  <si>
+    <t>OMIM</t>
+  </si>
+  <si>
+    <t>KEGG</t>
   </si>
 </sst>
 </file>
@@ -461,10 +464,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37AA32A1-06FE-4F2F-B1B3-BC04464E6BF0}">
-  <dimension ref="A1:Q1"/>
+  <dimension ref="A1:R1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="R2" sqref="R2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -482,15 +485,15 @@
     <col min="13" max="13" width="13.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>9</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>0</v>
@@ -511,28 +514,31 @@
         <v>3</v>
       </c>
       <c r="J1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>7</v>
-      </c>
       <c r="N1" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="O1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="P1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="P1" s="1" t="s">
-        <v>11</v>
-      </c>
       <c r="Q1" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -553,15 +559,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>